<commit_message>
0.6.9 ----- 	- Critical Fix : DLL crashed when not enough memory could be allocated. 	- Improved : Faster treaded access speed for Single Core machines 	- Improved : Speed increased ~20% when R/W small blocksizes (see benchmarks)
</commit_message>
<xml_diff>
--- a/Buffers/Benchmark/Benchmarks.xlsx
+++ b/Buffers/Benchmark/Benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>labels</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>v0.6.7</t>
+  </si>
+  <si>
+    <t>v0.6.9</t>
+  </si>
+  <si>
+    <t>v0.6.9 - 1 Channel</t>
+  </si>
+  <si>
+    <t>v0.6.9 - 32 Channels</t>
   </si>
 </sst>
 </file>
@@ -195,15 +204,15 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$2</c:f>
+              <c:f>Blad1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.4 - 1 Channel</c:v>
+                  <c:v>v0.6.9 - 32 Channels</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -211,148 +220,83 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$3:$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$3:$B$21</c:f>
+              <c:f>Blad1!$G$3:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8</c:v>
+                  <c:v>11.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.2</c:v>
+                  <c:v>21.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.2</c:v>
+                  <c:v>40.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.9</c:v>
+                  <c:v>80.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.7</c:v>
+                  <c:v>159.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>109</c:v>
+                  <c:v>309.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>121</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>143</c:v>
+                  <c:v>1090.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>149</c:v>
+                  <c:v>1981.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>150</c:v>
+                  <c:v>3512.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>150</c:v>
+                  <c:v>5661.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>169</c:v>
+                  <c:v>8143.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>167</c:v>
+                  <c:v>9861</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>168</c:v>
+                  <c:v>10940.9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>167</c:v>
+                  <c:v>11863.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>167</c:v>
+                  <c:v>12073.7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>167</c:v>
+                  <c:v>11291.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$C$2</c:f>
+              <c:f>Blad1!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.5 - 1 Channel</c:v>
+                  <c:v>v0.6.9 - 1 Channel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -360,282 +304,68 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$3:$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$3:$C$21</c:f>
+              <c:f>Blad1!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>4.7</c:v>
+                  <c:v>4.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>17.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>66.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>134.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124</c:v>
+                  <c:v>256.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>213</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>248</c:v>
+                  <c:v>911</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>288</c:v>
+                  <c:v>1574.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>313</c:v>
+                  <c:v>2749</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>325</c:v>
+                  <c:v>4647.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>336</c:v>
+                  <c:v>7145.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>339</c:v>
+                  <c:v>9589.7000000000007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>338</c:v>
+                  <c:v>11233.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>341</c:v>
+                  <c:v>11853</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>341</c:v>
+                  <c:v>12290</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>341</c:v>
+                  <c:v>12289</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>341</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7 - 1 Channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$3:$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$D$3:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>427</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>820</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1427</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2461</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4278</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6648</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9171</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11055</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11693</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12069</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12286</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11354</c:v>
+                  <c:v>11451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,7 +373,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$2</c:f>
@@ -725,12 +455,459 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.7 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$3:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1427</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2461</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4278</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6648</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9171</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11055</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11693</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12069</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12286</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.5 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$3:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.4 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100072448"/>
-        <c:axId val="101856384"/>
+        <c:axId val="101774464"/>
+        <c:axId val="101776768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100072448"/>
+        <c:axId val="101774464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,14 +932,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101856384"/>
+        <c:crossAx val="101776768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101856384"/>
+        <c:axId val="101776768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,7 +965,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100072448"/>
+        <c:crossAx val="101774464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -856,15 +1033,159 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$2</c:f>
+              <c:f>Blad1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.4 - 1 Channel</c:v>
+                  <c:v>v0.6.9 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159.30000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.9 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.7 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.7 - 1 Channel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -904,30 +1225,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$3:$B$9</c:f>
+              <c:f>Blad1!$D$3:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.2</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.2</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.9</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.7</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,7 +1256,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -1012,15 +1333,15 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$D$2</c:f>
+              <c:f>Blad1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.6.7 - 1 Channel</c:v>
+                  <c:v>v0.4 - 1 Channel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1060,89 +1381,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$D$3:$D$9</c:f>
+              <c:f>Blad1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>25.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>112</c:v>
+                  <c:v>43.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>217</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7 - 32 Channels</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$E$3:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>162</c:v>
+                  <c:v>60.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102409728"/>
-        <c:axId val="102411648"/>
+        <c:axId val="104806656"/>
+        <c:axId val="104841600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102409728"/>
+        <c:axId val="104806656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,14 +1441,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102411648"/>
+        <c:crossAx val="104841600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102411648"/>
+        <c:axId val="104841600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,7 +1474,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102409728"/>
+        <c:crossAx val="104806656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1291,15 +1564,183 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$24</c:f>
+              <c:f>Blad1!$E$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.4</c:v>
+                  <c:v>v0.6.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$38:$E$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>937</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1726</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4376</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5988</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8194</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9309</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$D$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$38:$D$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>258.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>937.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1726.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3122</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4376</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5988</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9309</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1309,7 +1750,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$25:$A$43</c:f>
+              <c:f>Blad1!$A$38:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -1374,81 +1815,81 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$25:$B$43</c:f>
+              <c:f>Blad1!$C$38:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>221</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>286</c:v>
+                  <c:v>574</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>287</c:v>
+                  <c:v>605</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>287</c:v>
+                  <c:v>606</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>286</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>320</c:v>
+                  <c:v>606</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>321</c:v>
+                  <c:v>604</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>320</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>322</c:v>
+                  <c:v>605</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>321</c:v>
+                  <c:v>605</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>319</c:v>
+                  <c:v>606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$C$24</c:f>
+              <c:f>Blad1!$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.5</c:v>
+                  <c:v>v0.4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1458,7 +1899,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$25:$A$43</c:f>
+              <c:f>Blad1!$A$38:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -1523,161 +1964,77 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$25:$C$43</c:f>
+              <c:f>Blad1!$B$38:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>179</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>246</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>427</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>495</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>574</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>605</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>606</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>607</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>606</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>604</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>607</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>605</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>605</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>606</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$D$25:$D$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131.30000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>258.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>501</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>937.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1726.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3122</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4376</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5988</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9309</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9394</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102462976"/>
-        <c:axId val="102464896"/>
+        <c:axId val="106773504"/>
+        <c:axId val="106783872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102462976"/>
+        <c:axId val="106773504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,14 +2059,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102464896"/>
+        <c:crossAx val="106783872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102464896"/>
+        <c:axId val="106783872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +2092,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102462976"/>
+        <c:crossAx val="106773504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1803,15 +2160,111 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$24</c:f>
+              <c:f>Blad1!$E$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.4</c:v>
+                  <c:v>v0.6.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$38:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$D$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.6.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$38:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>258.39999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1821,7 +2274,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Blad1!$A$25:$A$31</c:f>
+              <c:f>Blad1!$A$38:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1851,45 +2304,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$25:$B$31</c:f>
+              <c:f>Blad1!$C$38:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$C$24</c:f>
+              <c:f>Blad1!$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.5</c:v>
+                  <c:v>v0.4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1899,7 +2352,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Blad1!$A$25:$A$31</c:f>
+              <c:f>Blad1!$A$38:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1929,89 +2382,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$25:$C$31</c:f>
+              <c:f>Blad1!$B$38:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>179</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>246</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$D$25:$D$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131.30000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>258.39999999999998</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102635008"/>
-        <c:axId val="102636928"/>
+        <c:axId val="106483712"/>
+        <c:axId val="106485632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102635008"/>
+        <c:axId val="106483712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,14 +2442,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102636928"/>
+        <c:crossAx val="106485632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102636928"/>
+        <c:axId val="106485632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2475,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102635008"/>
+        <c:crossAx val="106483712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -2125,7 +2530,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2526,10 +2931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2538,6 +2943,8 @@
     <col min="2" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2564,8 +2971,12 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
@@ -2584,8 +2995,12 @@
       <c r="E3" s="1">
         <v>2.7</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="1">
+        <v>4.43</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.9</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
@@ -2604,8 +3019,12 @@
       <c r="E4" s="1">
         <v>5.3</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5.7</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
@@ -2624,8 +3043,12 @@
       <c r="E5" s="1">
         <v>10.7</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="1">
+        <v>17.34</v>
+      </c>
+      <c r="G5" s="1">
+        <v>11.21</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
@@ -2644,8 +3067,12 @@
       <c r="E6" s="1">
         <v>21</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1">
+        <v>21.3</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
@@ -2664,8 +3091,12 @@
       <c r="E7" s="1">
         <v>42</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1">
+        <v>66.7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>40.4</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
@@ -2684,8 +3115,12 @@
       <c r="E8" s="1">
         <v>84</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1">
+        <v>134.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>80.900000000000006</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
@@ -2704,8 +3139,12 @@
       <c r="E9" s="1">
         <v>162</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="1">
+        <v>256.3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>159.30000000000001</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
@@ -2724,8 +3163,12 @@
       <c r="E10" s="1">
         <v>322</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="1">
+        <v>513</v>
+      </c>
+      <c r="G10" s="1">
+        <v>309.5</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
@@ -2744,8 +3187,12 @@
       <c r="E11" s="1">
         <v>630</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1">
+        <v>911</v>
+      </c>
+      <c r="G11" s="1">
+        <v>608</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
@@ -2764,8 +3211,12 @@
       <c r="E12" s="1">
         <v>1103</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1">
+        <v>1574.6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1090.5999999999999</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
@@ -2784,8 +3235,12 @@
       <c r="E13" s="1">
         <v>2002</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="1">
+        <v>2749</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1981.6</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
@@ -2804,8 +3259,12 @@
       <c r="E14" s="1">
         <v>3554</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1">
+        <v>4647.3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3512.5</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
@@ -2824,8 +3283,12 @@
       <c r="E15" s="1">
         <v>5723</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1">
+        <v>7145.2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5661.4</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
@@ -2844,11 +3307,15 @@
       <c r="E16" s="1">
         <v>8268</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1">
+        <v>9589.7000000000007</v>
+      </c>
+      <c r="G16" s="1">
+        <v>8143.1</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -2864,11 +3331,15 @@
       <c r="E17" s="1">
         <v>9956</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1">
+        <v>11233.4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>9861</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -2884,11 +3355,15 @@
       <c r="E18" s="1">
         <v>10996</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="1">
+        <v>11853</v>
+      </c>
+      <c r="G18" s="1">
+        <v>10940.9</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -2904,11 +3379,15 @@
       <c r="E19" s="1">
         <v>11800</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="1">
+        <v>12290</v>
+      </c>
+      <c r="G19" s="1">
+        <v>11863.9</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -2924,11 +3403,15 @@
       <c r="E20" s="1">
         <v>12213</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="1">
+        <v>12289</v>
+      </c>
+      <c r="G20" s="1">
+        <v>12073.7</v>
+      </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -2944,284 +3427,30 @@
       <c r="E21" s="1">
         <v>11055</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="1">
+        <v>11451</v>
+      </c>
+      <c r="G21" s="1">
+        <v>11291.5</v>
+      </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="3" t="s">
+    <row r="37" spans="1:10">
+      <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4.3</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1">
-        <v>14.3</v>
-      </c>
-      <c r="D26" s="1">
-        <v>8.6</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1">
-        <v>12</v>
-      </c>
-      <c r="C27" s="1">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1">
-        <v>17</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1">
-        <v>69</v>
-      </c>
-      <c r="D28" s="1">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1">
-        <v>16</v>
-      </c>
-      <c r="B29" s="1">
-        <v>49</v>
-      </c>
-      <c r="C29" s="1">
-        <v>107</v>
-      </c>
-      <c r="D29" s="1">
-        <v>67.2</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1">
-        <v>32</v>
-      </c>
-      <c r="B30" s="1">
-        <v>88</v>
-      </c>
-      <c r="C30" s="1">
-        <v>179</v>
-      </c>
-      <c r="D30" s="1">
-        <v>131.30000000000001</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1">
-        <v>64</v>
-      </c>
-      <c r="B31" s="1">
-        <v>123</v>
-      </c>
-      <c r="C31" s="1">
-        <v>246</v>
-      </c>
-      <c r="D31" s="1">
-        <v>258.39999999999998</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1">
-        <v>128</v>
-      </c>
-      <c r="B32" s="1">
-        <v>221</v>
-      </c>
-      <c r="C32" s="1">
-        <v>427</v>
-      </c>
-      <c r="D32" s="1">
-        <v>501</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1">
-        <v>256</v>
-      </c>
-      <c r="B33" s="1">
-        <v>243</v>
-      </c>
-      <c r="C33" s="1">
-        <v>495</v>
-      </c>
-      <c r="D33" s="1">
-        <v>937.7</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1">
-        <v>512</v>
-      </c>
-      <c r="B34" s="1">
-        <v>286</v>
-      </c>
-      <c r="C34" s="1">
-        <v>574</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1726.8</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="1">
-        <v>287</v>
-      </c>
-      <c r="C35" s="1">
-        <v>605</v>
-      </c>
-      <c r="D35" s="1">
-        <v>3122</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="1">
-        <v>287</v>
-      </c>
-      <c r="C36" s="1">
-        <v>606</v>
-      </c>
-      <c r="D36" s="1">
-        <v>4376</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="1">
-        <v>286</v>
-      </c>
-      <c r="C37" s="1">
-        <v>607</v>
-      </c>
-      <c r="D37" s="1">
-        <v>5988</v>
-      </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -3229,19 +3458,21 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
+      <c r="A38" s="1">
+        <v>1</v>
       </c>
       <c r="B38" s="1">
-        <v>320</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1">
-        <v>606</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D38" s="1">
-        <v>8192</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>4.3</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -3249,19 +3480,21 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
+      <c r="A39" s="1">
+        <v>2</v>
       </c>
       <c r="B39" s="1">
-        <v>321</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1">
-        <v>604</v>
+        <v>14.3</v>
       </c>
       <c r="D39" s="1">
-        <v>9394</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>8.6</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10.1</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -3269,19 +3502,21 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="1" t="s">
-        <v>6</v>
+      <c r="A40" s="1">
+        <v>4</v>
       </c>
       <c r="B40" s="1">
-        <v>320</v>
+        <v>12</v>
       </c>
       <c r="C40" s="1">
-        <v>607</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1">
-        <v>9394</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E40" s="1">
+        <v>20.2</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -3289,19 +3524,21 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="1" t="s">
-        <v>7</v>
+      <c r="A41" s="1">
+        <v>8</v>
       </c>
       <c r="B41" s="1">
-        <v>322</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1">
-        <v>605</v>
+        <v>69</v>
       </c>
       <c r="D41" s="1">
-        <v>9394</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="E41" s="1">
+        <v>40</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -3309,19 +3546,21 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="1" t="s">
-        <v>8</v>
+      <c r="A42" s="1">
+        <v>16</v>
       </c>
       <c r="B42" s="1">
-        <v>321</v>
+        <v>49</v>
       </c>
       <c r="C42" s="1">
-        <v>605</v>
+        <v>107</v>
       </c>
       <c r="D42" s="1">
-        <v>9309</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>67.2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>67</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -3329,24 +3568,312 @@
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
-        <v>9</v>
+      <c r="A43" s="1">
+        <v>32</v>
       </c>
       <c r="B43" s="1">
-        <v>319</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1">
-        <v>606</v>
+        <v>179</v>
       </c>
       <c r="D43" s="1">
-        <v>9394</v>
-      </c>
-      <c r="E43" s="1"/>
+        <v>131.30000000000001</v>
+      </c>
+      <c r="E43" s="1">
+        <v>131.1</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
+        <v>64</v>
+      </c>
+      <c r="B44" s="1">
+        <v>123</v>
+      </c>
+      <c r="C44" s="1">
+        <v>246</v>
+      </c>
+      <c r="D44" s="1">
+        <v>258.39999999999998</v>
+      </c>
+      <c r="E44" s="1">
+        <v>257</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <v>128</v>
+      </c>
+      <c r="B45" s="1">
+        <v>221</v>
+      </c>
+      <c r="C45" s="1">
+        <v>427</v>
+      </c>
+      <c r="D45" s="1">
+        <v>501</v>
+      </c>
+      <c r="E45" s="1">
+        <v>498</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <v>256</v>
+      </c>
+      <c r="B46" s="1">
+        <v>243</v>
+      </c>
+      <c r="C46" s="1">
+        <v>495</v>
+      </c>
+      <c r="D46" s="1">
+        <v>937.7</v>
+      </c>
+      <c r="E46" s="1">
+        <v>937</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <v>512</v>
+      </c>
+      <c r="B47" s="1">
+        <v>286</v>
+      </c>
+      <c r="C47" s="1">
+        <v>574</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1726.8</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1726</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1">
+        <v>287</v>
+      </c>
+      <c r="C48" s="1">
+        <v>605</v>
+      </c>
+      <c r="D48" s="1">
+        <v>3122</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3121</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="1">
+        <v>287</v>
+      </c>
+      <c r="C49" s="1">
+        <v>606</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4376</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4376</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="1">
+        <v>286</v>
+      </c>
+      <c r="C50" s="1">
+        <v>607</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5988</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5988</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>320</v>
+      </c>
+      <c r="C51" s="1">
+        <v>606</v>
+      </c>
+      <c r="D51" s="1">
+        <v>8192</v>
+      </c>
+      <c r="E51" s="1">
+        <v>8194</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
+        <v>321</v>
+      </c>
+      <c r="C52" s="1">
+        <v>604</v>
+      </c>
+      <c r="D52" s="1">
+        <v>9394</v>
+      </c>
+      <c r="E52" s="1">
+        <v>9309</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1">
+        <v>320</v>
+      </c>
+      <c r="C53" s="1">
+        <v>607</v>
+      </c>
+      <c r="D53" s="1">
+        <v>9394</v>
+      </c>
+      <c r="E53" s="1">
+        <v>9394</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1">
+        <v>322</v>
+      </c>
+      <c r="C54" s="1">
+        <v>605</v>
+      </c>
+      <c r="D54" s="1">
+        <v>9394</v>
+      </c>
+      <c r="E54" s="1">
+        <v>9394</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1">
+        <v>321</v>
+      </c>
+      <c r="C55" s="1">
+        <v>605</v>
+      </c>
+      <c r="D55" s="1">
+        <v>9309</v>
+      </c>
+      <c r="E55" s="1">
+        <v>9394</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="1">
+        <v>319</v>
+      </c>
+      <c r="C56" s="1">
+        <v>606</v>
+      </c>
+      <c r="D56" s="1">
+        <v>9394</v>
+      </c>
+      <c r="E56" s="1">
+        <v>9394</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
0.7.0 ----- 	- Changed : Renamed project files from "Buffers.xxx" to "UltraQueue.xxx" :) 	- Fix : BufferCreate() could cause a mem. access violation in very specific low memory environments. 	- Added : BufferCreate() could return 0 for multiple reasons. 		  new param. (*Status) was added for error handling. (See "UltraQueue.h" for details) 	- Improved : Finetuned highly threaded access with small blocksizes (~280% speed improvement) 	- Improved : Improved Threaded performance for HyperThreading-enabled CPU's 	- Improved : CPU load decreased in high-threaded situations (~50%) 	- Improved : Queue access latency lowered by ~35% in specific high threaded situations. 	- Improved : Slightly optimized clean-up code on queue creating errors. 	- Changed : Code Example file has been updated with new parameter in BufferCreate().
	- Added : Benchmark application (Needs .NET 4.0 x86)
</commit_message>
<xml_diff>
--- a/Buffers/Benchmark/Benchmarks.xlsx
+++ b/Buffers/Benchmark/Benchmarks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>labels</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>v0.6.9 - 32 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.0 - 1 Channel</t>
+  </si>
+  <si>
+    <t>v0.7.0</t>
   </si>
 </sst>
 </file>
@@ -204,8 +210,92 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.0 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$3:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2409</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3241</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4930</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7291</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12972</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12962</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11546</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -289,7 +379,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -373,7 +463,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$2</c:f>
@@ -457,7 +547,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$D$2</c:f>
@@ -606,7 +696,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -755,7 +845,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$B$2</c:f>
@@ -903,11 +993,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101774464"/>
-        <c:axId val="101776768"/>
+        <c:axId val="99745152"/>
+        <c:axId val="99751808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101774464"/>
+        <c:axId val="99745152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,14 +1022,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101776768"/>
+        <c:crossAx val="99751808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101776768"/>
+        <c:axId val="99751808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +1055,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101774464"/>
+        <c:crossAx val="99745152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1033,8 +1123,56 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.0 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -1082,7 +1220,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -1130,7 +1268,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$2</c:f>
@@ -1178,7 +1316,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$D$2</c:f>
@@ -1256,7 +1394,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -1334,7 +1472,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$B$2</c:f>
@@ -1411,11 +1549,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104806656"/>
-        <c:axId val="104841600"/>
+        <c:axId val="101047296"/>
+        <c:axId val="101053568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104806656"/>
+        <c:axId val="101047296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,14 +1579,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104841600"/>
+        <c:crossAx val="101053568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104841600"/>
+        <c:axId val="101053568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,10 +1612,10 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104806656"/>
+        <c:crossAx val="101047296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="50"/>
         <c:minorUnit val="10"/>
       </c:valAx>
     </c:plotArea>
@@ -1564,8 +1702,92 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$F$38:$F$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2737</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6564</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8258</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11130</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10893</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -1649,7 +1871,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$D$37</c:f>
@@ -1733,7 +1955,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$37</c:f>
@@ -1882,7 +2104,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$B$37</c:f>
@@ -2030,11 +2252,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106773504"/>
-        <c:axId val="106783872"/>
+        <c:axId val="101118720"/>
+        <c:axId val="101120640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106773504"/>
+        <c:axId val="101118720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2059,14 +2281,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106783872"/>
+        <c:crossAx val="101120640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106783872"/>
+        <c:axId val="101120640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,7 +2314,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106773504"/>
+        <c:crossAx val="101118720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -2160,8 +2382,56 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$F$38:$F$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1026</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -2209,7 +2479,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$D$37</c:f>
@@ -2257,7 +2527,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$37</c:f>
@@ -2335,7 +2605,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$B$37</c:f>
@@ -2412,11 +2682,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106483712"/>
-        <c:axId val="106485632"/>
+        <c:axId val="101533952"/>
+        <c:axId val="101560704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106483712"/>
+        <c:axId val="101533952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,14 +2712,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106485632"/>
+        <c:crossAx val="101560704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106485632"/>
+        <c:axId val="101560704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2475,10 +2745,10 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106483712"/>
+        <c:crossAx val="101533952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2934,7 +3204,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2945,9 +3215,10 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2955,7 +3226,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2977,9 +3248,11 @@
       <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3001,9 +3274,12 @@
       <c r="G3" s="1">
         <v>2.9</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3025,9 +3301,12 @@
       <c r="G4" s="1">
         <v>5.7</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3049,9 +3328,12 @@
       <c r="G5" s="1">
         <v>11.21</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>55</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -3073,9 +3355,12 @@
       <c r="G6" s="1">
         <v>21.3</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -3097,9 +3382,12 @@
       <c r="G7" s="1">
         <v>40.4</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>210</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -3121,9 +3409,12 @@
       <c r="G8" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>410</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -3145,9 +3436,12 @@
       <c r="G9" s="1">
         <v>159.30000000000001</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>744</v>
+      </c>
+      <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>128</v>
       </c>
@@ -3169,9 +3463,12 @@
       <c r="G10" s="1">
         <v>309.5</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1368</v>
+      </c>
+      <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>256</v>
       </c>
@@ -3193,9 +3490,12 @@
       <c r="G11" s="1">
         <v>608</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>2409</v>
+      </c>
+      <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>512</v>
       </c>
@@ -3217,9 +3517,12 @@
       <c r="G12" s="1">
         <v>1090.5999999999999</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>3241</v>
+      </c>
+      <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3241,9 +3544,12 @@
       <c r="G13" s="1">
         <v>1981.6</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>4930</v>
+      </c>
+      <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -3265,9 +3571,12 @@
       <c r="G14" s="1">
         <v>3512.5</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>7291</v>
+      </c>
+      <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3289,9 +3598,12 @@
       <c r="G15" s="1">
         <v>5661.4</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>11932</v>
+      </c>
+      <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -3313,9 +3625,12 @@
       <c r="G16" s="1">
         <v>8143.1</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>12972</v>
+      </c>
+      <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -3337,9 +3652,12 @@
       <c r="G17" s="1">
         <v>9861</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>12962</v>
+      </c>
+      <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3361,9 +3679,12 @@
       <c r="G18" s="1">
         <v>10940.9</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>12497</v>
+      </c>
+      <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3385,9 +3706,12 @@
       <c r="G19" s="1">
         <v>11863.9</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>12810</v>
+      </c>
+      <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3409,9 +3733,12 @@
       <c r="G20" s="1">
         <v>12073.7</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1">
+        <v>12497</v>
+      </c>
+      <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -3433,7 +3760,10 @@
       <c r="G21" s="1">
         <v>11291.5</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>11546</v>
+      </c>
+      <c r="I21" s="1"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
@@ -3451,7 +3781,9 @@
       <c r="E37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -3473,7 +3805,9 @@
       <c r="E38" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1">
+        <v>19</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -3495,7 +3829,9 @@
       <c r="E39" s="1">
         <v>10.1</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39" s="1">
+        <v>38</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -3517,7 +3853,9 @@
       <c r="E40" s="1">
         <v>20.2</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1">
+        <v>73</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -3539,7 +3877,9 @@
       <c r="E41" s="1">
         <v>40</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1">
+        <v>127</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -3561,7 +3901,9 @@
       <c r="E42" s="1">
         <v>67</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1">
+        <v>285</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3583,7 +3925,9 @@
       <c r="E43" s="1">
         <v>131.1</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1">
+        <v>529</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3605,7 +3949,9 @@
       <c r="E44" s="1">
         <v>257</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1">
+        <v>1026</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -3627,7 +3973,9 @@
       <c r="E45" s="1">
         <v>498</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1">
+        <v>1822</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -3649,7 +3997,9 @@
       <c r="E46" s="1">
         <v>937</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1">
+        <v>2737</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -3671,7 +4021,9 @@
       <c r="E47" s="1">
         <v>1726</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="1">
+        <v>4096</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -3693,7 +4045,9 @@
       <c r="E48" s="1">
         <v>3121</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48" s="1">
+        <v>6564</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -3715,7 +4069,9 @@
       <c r="E49" s="1">
         <v>4376</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49" s="1">
+        <v>8258</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -3737,7 +4093,9 @@
       <c r="E50" s="1">
         <v>5988</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1">
+        <v>10893</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -3759,7 +4117,9 @@
       <c r="E51" s="1">
         <v>8194</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51" s="1">
+        <v>10893</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -3781,7 +4141,9 @@
       <c r="E52" s="1">
         <v>9309</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52" s="1">
+        <v>10893</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -3803,7 +4165,9 @@
       <c r="E53" s="1">
         <v>9394</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1">
+        <v>10893</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -3825,7 +4189,9 @@
       <c r="E54" s="1">
         <v>9394</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1">
+        <v>10893</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -3847,7 +4213,9 @@
       <c r="E55" s="1">
         <v>9394</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="1">
+        <v>11130</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -3869,7 +4237,9 @@
       <c r="E56" s="1">
         <v>9394</v>
       </c>
-      <c r="F56" s="1"/>
+      <c r="F56" s="1">
+        <v>10893</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>

</xml_diff>

<commit_message>
0.7.1 ----- 	- Fix : BufferRead() could never return "-3" (Queue is Empty), even if it was empty. 	- Improved : Updated max nr of Read Channels from 32 to 128. 		     keep in mind that every additional Read Channel costs a little bit extra CPU power. 		     See benchmarks for details. 		     It's advised to not make more ReadChannels than you need, in order to have max performance.
</commit_message>
<xml_diff>
--- a/Buffers/Benchmark/Benchmarks.xlsx
+++ b/Buffers/Benchmark/Benchmarks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>labels</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>v0.7.0</t>
+  </si>
+  <si>
+    <t>v.0.7.1 - 1 Channel</t>
+  </si>
+  <si>
+    <t>v.0.7.1 - 32 Channels</t>
+  </si>
+  <si>
+    <t>v0.7.1</t>
+  </si>
+  <si>
+    <t>v.0.7.1 - 128 Channels</t>
   </si>
 </sst>
 </file>
@@ -210,8 +222,260 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$K$3:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1539</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2807</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4753</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7195</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10502</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11669</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12073</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11175</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$J$3:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1145</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3173</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5251</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7839</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10195</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11538</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11804</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11546</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$3:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2365</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4890</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7243</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11870</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12972</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12496</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="6"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -295,7 +559,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -379,7 +643,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -462,99 +726,15 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="1"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$E$2</c:f>
+              <c:f>Blad1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.6.7 - 32 Channels</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$E$3:$E$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>630</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1103</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3554</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5723</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8268</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9956</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12213</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11055</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7 - 1 Channel</c:v>
+                  <c:v>v0.5 - 1 Channel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -629,155 +809,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$D$3:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>427</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>820</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1427</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2461</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4278</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6648</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9171</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11055</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11693</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12069</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12286</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11354</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.5 - 1 Channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$3:$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Blad1!$C$3:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -838,166 +869,17 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>341</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.4 - 1 Channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$3:$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$B$3:$B$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>149</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99745152"/>
-        <c:axId val="99751808"/>
+        <c:axId val="82500992"/>
+        <c:axId val="99030912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99745152"/>
+        <c:axId val="82500992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,14 +904,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99751808"/>
+        <c:crossAx val="99030912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99751808"/>
+        <c:axId val="99030912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +937,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99745152"/>
+        <c:crossAx val="82500992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1123,8 +1005,152 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$K$3:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.1 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="6"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -1172,7 +1198,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -1220,7 +1246,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -1267,63 +1293,15 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="1"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$E$2</c:f>
+              <c:f>Blad1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v0.6.7 - 32 Channels</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$E$3:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>162</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7 - 1 Channel</c:v>
+                  <c:v>v0.5 - 1 Channel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1363,84 +1341,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$D$3:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>217</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.5 - 1 Channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Blad1!$A$3:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Blad1!$C$3:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1465,95 +1365,17 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>124</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.4 - 1 Channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Blad1!$A$3:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$B$3:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101047296"/>
-        <c:axId val="101053568"/>
+        <c:axId val="100588544"/>
+        <c:axId val="100594816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101047296"/>
+        <c:axId val="100588544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,14 +1401,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101053568"/>
+        <c:crossAx val="100594816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101053568"/>
+        <c:axId val="100594816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,7 +1434,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101047296"/>
+        <c:crossAx val="100588544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1702,8 +1524,92 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$G$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$38:$G$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2976</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4697</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6564</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8258</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11129</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10893</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="4"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$37</c:f>
@@ -1787,7 +1693,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -1870,90 +1776,6 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$D$38:$D$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131.30000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>258.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>501</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>937.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1726.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3122</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4376</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5988</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9394</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9309</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9394</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="3"/>
           <c:tx>
@@ -2102,161 +1924,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$B$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Blad1!$A$38:$A$56</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1k</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2k</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4k</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8k</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16k</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32k</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64k</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>128k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$B$38:$B$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>243</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>286</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>287</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>287</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>286</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>321</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>321</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>319</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101118720"/>
-        <c:axId val="101120640"/>
+        <c:axId val="100913920"/>
+        <c:axId val="100915840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101118720"/>
+        <c:axId val="100913920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2281,14 +1954,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101120640"/>
+        <c:crossAx val="100915840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101120640"/>
+        <c:axId val="100915840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2314,7 +1987,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101118720"/>
+        <c:crossAx val="100913920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -2382,8 +2055,56 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$G$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$38:$G$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="4"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$37</c:f>
@@ -2431,7 +2152,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -2478,54 +2199,6 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$D$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.6.7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$D$38:$D$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131.30000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>258.39999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="3"/>
           <c:tx>
@@ -2603,90 +2276,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Blad1!$B$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>v0.4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Blad1!$A$38:$A$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Blad1!$B$38:$B$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>123</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101533952"/>
-        <c:axId val="101560704"/>
+        <c:axId val="101583104"/>
+        <c:axId val="101622144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101533952"/>
+        <c:axId val="101583104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2712,14 +2307,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101560704"/>
+        <c:crossAx val="101622144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101560704"/>
+        <c:axId val="101622144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2745,7 +2340,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101533952"/>
+        <c:crossAx val="101583104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -2764,7 +2359,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2776,7 +2371,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3201,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3215,10 +2810,12 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -3226,7 +2823,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3251,8 +2848,17 @@
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3277,9 +2883,17 @@
       <c r="H3" s="1">
         <v>15</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3304,9 +2918,17 @@
       <c r="H4" s="1">
         <v>29</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="J4" s="1">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3331,9 +2953,17 @@
       <c r="H5" s="1">
         <v>55</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <v>53</v>
+      </c>
+      <c r="J5" s="1">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -3358,9 +2988,17 @@
       <c r="H6" s="1">
         <v>100</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <v>98</v>
+      </c>
+      <c r="J6" s="1">
+        <v>38</v>
+      </c>
+      <c r="K6" s="1">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -3385,9 +3023,17 @@
       <c r="H7" s="1">
         <v>210</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>205</v>
+      </c>
+      <c r="J7" s="1">
+        <v>78</v>
+      </c>
+      <c r="K7" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -3412,9 +3058,17 @@
       <c r="H8" s="1">
         <v>410</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <v>403</v>
+      </c>
+      <c r="J8" s="1">
+        <v>156</v>
+      </c>
+      <c r="K8" s="1">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -3439,9 +3093,17 @@
       <c r="H9" s="1">
         <v>744</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <v>739</v>
+      </c>
+      <c r="J9" s="1">
+        <v>308</v>
+      </c>
+      <c r="K9" s="1">
+        <v>119</v>
+      </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>128</v>
       </c>
@@ -3466,9 +3128,17 @@
       <c r="H10" s="1">
         <v>1368</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1">
+        <v>1360</v>
+      </c>
+      <c r="J10" s="1">
+        <v>598</v>
+      </c>
+      <c r="K10" s="1">
+        <v>236</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>256</v>
       </c>
@@ -3493,9 +3163,17 @@
       <c r="H11" s="1">
         <v>2409</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>2365</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1145</v>
+      </c>
+      <c r="K11" s="1">
+        <v>461</v>
+      </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>512</v>
       </c>
@@ -3520,9 +3198,17 @@
       <c r="H12" s="1">
         <v>3241</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>3213</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1855</v>
+      </c>
+      <c r="K12" s="1">
+        <v>833</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3547,9 +3233,17 @@
       <c r="H13" s="1">
         <v>4930</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>4890</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3173</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1539</v>
+      </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -3574,9 +3268,17 @@
       <c r="H14" s="1">
         <v>7291</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>7243</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5251</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2807</v>
+      </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3601,9 +3303,17 @@
       <c r="H15" s="1">
         <v>11932</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <v>11870</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7839</v>
+      </c>
+      <c r="K15" s="1">
+        <v>4753</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -3628,9 +3338,17 @@
       <c r="H16" s="1">
         <v>12972</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1">
+        <v>12972</v>
+      </c>
+      <c r="J16" s="1">
+        <v>10195</v>
+      </c>
+      <c r="K16" s="1">
+        <v>7195</v>
+      </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -3655,9 +3373,17 @@
       <c r="H17" s="1">
         <v>12962</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>12960</v>
+      </c>
+      <c r="J17" s="1">
+        <v>11538</v>
+      </c>
+      <c r="K17" s="1">
+        <v>8899</v>
+      </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3682,9 +3408,17 @@
       <c r="H18" s="1">
         <v>12497</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <v>12496</v>
+      </c>
+      <c r="J18" s="1">
+        <v>11804</v>
+      </c>
+      <c r="K18" s="1">
+        <v>10502</v>
+      </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3709,9 +3443,17 @@
       <c r="H19" s="1">
         <v>12810</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>12810</v>
+      </c>
+      <c r="J19" s="1">
+        <v>12355</v>
+      </c>
+      <c r="K19" s="1">
+        <v>11669</v>
+      </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3736,9 +3478,17 @@
       <c r="H20" s="1">
         <v>12497</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>12497</v>
+      </c>
+      <c r="J20" s="1">
+        <v>12355</v>
+      </c>
+      <c r="K20" s="1">
+        <v>12073</v>
+      </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -3763,7 +3513,15 @@
       <c r="H21" s="1">
         <v>11546</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1">
+        <v>11669</v>
+      </c>
+      <c r="J21" s="1">
+        <v>11546</v>
+      </c>
+      <c r="K21" s="1">
+        <v>11175</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
@@ -3784,7 +3542,9 @@
       <c r="F37" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="1"/>
+      <c r="G37" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -3808,7 +3568,9 @@
       <c r="F38" s="1">
         <v>19</v>
       </c>
-      <c r="G38" s="1"/>
+      <c r="G38" s="1">
+        <v>22</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -3832,7 +3594,9 @@
       <c r="F39" s="1">
         <v>38</v>
       </c>
-      <c r="G39" s="1"/>
+      <c r="G39" s="1">
+        <v>42</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -3856,7 +3620,9 @@
       <c r="F40" s="1">
         <v>73</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="1">
+        <v>80</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -3880,7 +3646,9 @@
       <c r="F41" s="1">
         <v>127</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1">
+        <v>142</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -3904,7 +3672,9 @@
       <c r="F42" s="1">
         <v>285</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1">
+        <v>306</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3928,7 +3698,9 @@
       <c r="F43" s="1">
         <v>529</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1">
+        <v>528</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3952,7 +3724,9 @@
       <c r="F44" s="1">
         <v>1026</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1">
+        <v>1024</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3976,7 +3750,9 @@
       <c r="F45" s="1">
         <v>1822</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1">
+        <v>1828</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -4000,7 +3776,9 @@
       <c r="F46" s="1">
         <v>2737</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1">
+        <v>2976</v>
+      </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -4024,7 +3802,9 @@
       <c r="F47" s="1">
         <v>4096</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="1">
+        <v>4697</v>
+      </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -4048,7 +3828,9 @@
       <c r="F48" s="1">
         <v>6564</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="1">
+        <v>6564</v>
+      </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -4072,7 +3854,9 @@
       <c r="F49" s="1">
         <v>8258</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49" s="1">
+        <v>8258</v>
+      </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -4096,7 +3880,9 @@
       <c r="F50" s="1">
         <v>10893</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50" s="1">
+        <v>10893</v>
+      </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -4120,7 +3906,9 @@
       <c r="F51" s="1">
         <v>10893</v>
       </c>
-      <c r="G51" s="1"/>
+      <c r="G51" s="1">
+        <v>10893</v>
+      </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -4144,7 +3932,9 @@
       <c r="F52" s="1">
         <v>10893</v>
       </c>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1">
+        <v>10893</v>
+      </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -4168,7 +3958,9 @@
       <c r="F53" s="1">
         <v>10893</v>
       </c>
-      <c r="G53" s="1"/>
+      <c r="G53" s="1">
+        <v>10893</v>
+      </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -4192,7 +3984,9 @@
       <c r="F54" s="1">
         <v>10893</v>
       </c>
-      <c r="G54" s="1"/>
+      <c r="G54" s="1">
+        <v>10893</v>
+      </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -4216,7 +4010,9 @@
       <c r="F55" s="1">
         <v>11130</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1">
+        <v>11129</v>
+      </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -4240,7 +4036,9 @@
       <c r="F56" s="1">
         <v>10893</v>
       </c>
-      <c r="G56" s="1"/>
+      <c r="G56" s="1">
+        <v>10893</v>
+      </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>

</xml_diff>

<commit_message>
0.7.2 ----- 	- Critical Fix : Queue data could get corrupt after lots of reading/writing. 	- Improved : ~13% speed gain on small writes when using a lot of channels. 	- Improved : ~15% speed gain when writing data to a full FIFO queue. 	- Improved : ~60% speed gain when Flushing all ReadChannels at once (using "-1" in the command) 	- Changed : BufferGetOverflow_Wait(BufferNr) returns an Unsigned Int now i.s.o. a Bool. (compatibility with ANSI C) 	- Updated : Write Benchmarks & Code Example
</commit_message>
<xml_diff>
--- a/Buffers/Benchmark/Benchmarks.xlsx
+++ b/Buffers/Benchmark/Benchmarks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>labels</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>v.0.7.1 - 128 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.2 - 1 Channel</t>
+  </si>
+  <si>
+    <t>v.0.7.2 - 32 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.2 - 128 Channels</t>
   </si>
 </sst>
 </file>
@@ -222,8 +231,176 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="8"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$N$3:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1569</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4840</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7294</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9051</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10502</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11669</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12073</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11291</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$M$3:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1916</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3302</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5414</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7957</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10297</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11538</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11795</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$K$2</c:f>
@@ -307,7 +484,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$J$2</c:f>
@@ -391,7 +568,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$I$2</c:f>
@@ -475,7 +652,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -559,7 +736,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="4"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -643,7 +820,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -727,7 +904,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="6"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -875,11 +1052,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82500992"/>
-        <c:axId val="99030912"/>
+        <c:axId val="101707136"/>
+        <c:axId val="101975936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82500992"/>
+        <c:axId val="101707136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,14 +1081,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99030912"/>
+        <c:crossAx val="101975936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99030912"/>
+        <c:axId val="101975936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +1114,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82500992"/>
+        <c:crossAx val="101707136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1005,8 +1182,104 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="8"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$N$3:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$M$3:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$K$2</c:f>
@@ -1054,7 +1327,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$J$2</c:f>
@@ -1102,7 +1375,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$I$2</c:f>
@@ -1150,7 +1423,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -1198,7 +1471,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="4"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -1246,7 +1519,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="5"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -1294,7 +1567,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="6"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -1371,11 +1644,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100588544"/>
-        <c:axId val="100594816"/>
+        <c:axId val="103074816"/>
+        <c:axId val="103081088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100588544"/>
+        <c:axId val="103074816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,14 +1674,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100594816"/>
+        <c:crossAx val="103081088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100594816"/>
+        <c:axId val="103081088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,7 +1707,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100588544"/>
+        <c:crossAx val="103074816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1517,7 +1790,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1925,11 +2197,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100913920"/>
-        <c:axId val="100915840"/>
+        <c:axId val="103411712"/>
+        <c:axId val="103413632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100913920"/>
+        <c:axId val="103411712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,18 +2222,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100915840"/>
+        <c:crossAx val="103413632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100915840"/>
+        <c:axId val="103413632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,11 +2254,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100913920"/>
+        <c:crossAx val="103411712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1995,7 +2265,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2048,7 +2317,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2277,11 +2545,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101583104"/>
-        <c:axId val="101622144"/>
+        <c:axId val="103568128"/>
+        <c:axId val="103570048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101583104"/>
+        <c:axId val="103568128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,19 +2570,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101622144"/>
+        <c:crossAx val="103570048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101622144"/>
+        <c:axId val="103570048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2336,11 +2603,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101583104"/>
+        <c:crossAx val="103568128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -2348,7 +2614,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2359,7 +2624,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2371,7 +2636,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2796,10 +3061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2813,9 +3078,12 @@
     <col min="8" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2823,7 +3091,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2857,8 +3125,17 @@
       <c r="K2" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2892,8 +3169,17 @@
       <c r="K3" s="1">
         <v>1</v>
       </c>
+      <c r="L3" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2927,8 +3213,17 @@
       <c r="K4" s="1">
         <v>3</v>
       </c>
+      <c r="L4" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="M4" s="1">
+        <v>12</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2962,8 +3257,17 @@
       <c r="K5" s="1">
         <v>7</v>
       </c>
+      <c r="L5" s="1">
+        <v>53</v>
+      </c>
+      <c r="M5" s="1">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -2997,8 +3301,17 @@
       <c r="K6" s="1">
         <v>14</v>
       </c>
+      <c r="L6" s="1">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1">
+        <v>44</v>
+      </c>
+      <c r="N6" s="1">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -3032,8 +3345,17 @@
       <c r="K7" s="1">
         <v>30</v>
       </c>
+      <c r="L7" s="1">
+        <v>205</v>
+      </c>
+      <c r="M7" s="1">
+        <v>92</v>
+      </c>
+      <c r="N7" s="1">
+        <v>31</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -3067,8 +3389,17 @@
       <c r="K8" s="1">
         <v>60</v>
       </c>
+      <c r="L8" s="1">
+        <v>403</v>
+      </c>
+      <c r="M8" s="1">
+        <v>184</v>
+      </c>
+      <c r="N8" s="1">
+        <v>63</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -3102,8 +3433,17 @@
       <c r="K9" s="1">
         <v>119</v>
       </c>
+      <c r="L9" s="1">
+        <v>739</v>
+      </c>
+      <c r="M9" s="1">
+        <v>344</v>
+      </c>
+      <c r="N9" s="1">
+        <v>121</v>
+      </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>128</v>
       </c>
@@ -3137,8 +3477,17 @@
       <c r="K10" s="1">
         <v>236</v>
       </c>
+      <c r="L10" s="1">
+        <v>1360</v>
+      </c>
+      <c r="M10" s="1">
+        <v>668</v>
+      </c>
+      <c r="N10" s="1">
+        <v>239</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>256</v>
       </c>
@@ -3172,8 +3521,17 @@
       <c r="K11" s="1">
         <v>461</v>
       </c>
+      <c r="L11" s="1">
+        <v>2365</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1253</v>
+      </c>
+      <c r="N11" s="1">
+        <v>466</v>
+      </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>512</v>
       </c>
@@ -3207,8 +3565,17 @@
       <c r="K12" s="1">
         <v>833</v>
       </c>
+      <c r="L12" s="1">
+        <v>3213</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1916</v>
+      </c>
+      <c r="N12" s="1">
+        <v>846</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3242,8 +3609,17 @@
       <c r="K13" s="1">
         <v>1539</v>
       </c>
+      <c r="L13" s="1">
+        <v>4890</v>
+      </c>
+      <c r="M13" s="1">
+        <v>3302</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1569</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -3277,8 +3653,17 @@
       <c r="K14" s="1">
         <v>2807</v>
       </c>
+      <c r="L14" s="1">
+        <v>7243</v>
+      </c>
+      <c r="M14" s="1">
+        <v>5414</v>
+      </c>
+      <c r="N14" s="1">
+        <v>2831</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3312,8 +3697,17 @@
       <c r="K15" s="1">
         <v>4753</v>
       </c>
+      <c r="L15" s="1">
+        <v>11870</v>
+      </c>
+      <c r="M15" s="1">
+        <v>7957</v>
+      </c>
+      <c r="N15" s="1">
+        <v>4840</v>
+      </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -3347,8 +3741,17 @@
       <c r="K16" s="1">
         <v>7195</v>
       </c>
+      <c r="L16" s="1">
+        <v>12972</v>
+      </c>
+      <c r="M16" s="1">
+        <v>10297</v>
+      </c>
+      <c r="N16" s="1">
+        <v>7294</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -3382,8 +3785,17 @@
       <c r="K17" s="1">
         <v>8899</v>
       </c>
+      <c r="L17" s="1">
+        <v>12960</v>
+      </c>
+      <c r="M17" s="1">
+        <v>11538</v>
+      </c>
+      <c r="N17" s="1">
+        <v>9051</v>
+      </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3417,8 +3829,17 @@
       <c r="K18" s="1">
         <v>10502</v>
       </c>
+      <c r="L18" s="1">
+        <v>12496</v>
+      </c>
+      <c r="M18" s="1">
+        <v>11795</v>
+      </c>
+      <c r="N18" s="1">
+        <v>10502</v>
+      </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3452,8 +3873,17 @@
       <c r="K19" s="1">
         <v>11669</v>
       </c>
+      <c r="L19" s="1">
+        <v>12810</v>
+      </c>
+      <c r="M19" s="1">
+        <v>12208</v>
+      </c>
+      <c r="N19" s="1">
+        <v>11669</v>
+      </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3487,8 +3917,17 @@
       <c r="K20" s="1">
         <v>12073</v>
       </c>
+      <c r="L20" s="1">
+        <v>12497</v>
+      </c>
+      <c r="M20" s="1">
+        <v>12355</v>
+      </c>
+      <c r="N20" s="1">
+        <v>12073</v>
+      </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -3521,6 +3960,15 @@
       </c>
       <c r="K21" s="1">
         <v>11175</v>
+      </c>
+      <c r="L21" s="1">
+        <v>11669</v>
+      </c>
+      <c r="M21" s="1">
+        <v>11417</v>
+      </c>
+      <c r="N21" s="1">
+        <v>11291</v>
       </c>
     </row>
     <row r="37" spans="1:10">

</xml_diff>

<commit_message>
0.7.3 ----- 	- Improved : Queue access functions dynamically select the fastest possible method for any situation now. 	- Improved : Fully optimized cache performance. 	- Improved : Read/Write performance fully optimized on assembly level. (See benchmarks for details) 	- Improved : Vectorized Load & Pointer handling, improving queue performance when using High Readpointer count. 	- Improved : ReWritten CPU info functions in Assembly now for extremely fast Queue creation & control 	- Improved : Seriously improved pointer aliasing, false sharing & boundary alignments for optimal caching & SSE2 performance. 	- Improved : Read/Writes smaller than 4kB are now handled by Agner Fog's "Asmlib" memcpy functions. 		     (Special Thanks to Agner Fog for the amazing optimization manuals & libs !! - please visit www.agner.org) 	- Updated : All benchmarks 	- Added : Comparison Benchmarks based on Queue sizes fitting in RAM, L2 & L1 cache.
</commit_message>
<xml_diff>
--- a/Buffers/Benchmark/Benchmarks.xlsx
+++ b/Buffers/Benchmark/Benchmarks.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Grafiek1" sheetId="5" r:id="rId2"/>
-    <sheet name="Grafiek2" sheetId="7" r:id="rId3"/>
-    <sheet name="Grafiek3" sheetId="8" r:id="rId4"/>
-    <sheet name="Grafiek4" sheetId="9" r:id="rId5"/>
+    <sheet name="Grafiek 1_2" sheetId="10" r:id="rId3"/>
+    <sheet name="Grafiek 1_Cache" sheetId="12" r:id="rId4"/>
+    <sheet name="Grafiek2" sheetId="7" r:id="rId5"/>
+    <sheet name="Grafiek2 (2)" sheetId="11" r:id="rId6"/>
+    <sheet name="Grafiek3" sheetId="8" r:id="rId7"/>
+    <sheet name="Grafiek4" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>labels</t>
   </si>
@@ -111,6 +114,30 @@
   </si>
   <si>
     <t>v.0.7.2 - 128 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 1 Channel</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 32 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 128 Channels</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 1Ch - 256MB - RAM</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 1Ch - 16kB - (L1 Cache / 2)</t>
+  </si>
+  <si>
+    <t>v.0.7.3 - 1Ch - 128kB - (L2 Cache / 2)</t>
+  </si>
+  <si>
+    <t>v0.7.2</t>
+  </si>
+  <si>
+    <t>v0.7.3</t>
   </si>
 </sst>
 </file>
@@ -231,8 +258,260 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="11"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$Q$3:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1157</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9816</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11055</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12217</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$P$3:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3646</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5868</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8609</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10937</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12506</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$O$3:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2846</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4861</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8266</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12962</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12651</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="8"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$N$2</c:f>
@@ -316,7 +595,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$M$2</c:f>
@@ -399,8 +678,92 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="12"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$L$3:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2365</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4890</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7243</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11870</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12972</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12496</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$K$2</c:f>
@@ -484,7 +847,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$J$2</c:f>
@@ -568,7 +931,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="4"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$I$2</c:f>
@@ -652,7 +1015,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="5"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -736,7 +1099,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="6"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -820,7 +1183,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="7"/>
+          <c:order val="11"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -904,7 +1267,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="8"/>
+          <c:order val="12"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -1052,11 +1415,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101707136"/>
-        <c:axId val="101975936"/>
+        <c:axId val="102282368"/>
+        <c:axId val="102284672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101707136"/>
+        <c:axId val="102282368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,14 +1444,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101975936"/>
+        <c:crossAx val="102284672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101975936"/>
+        <c:axId val="102284672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1477,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101707136"/>
+        <c:crossAx val="102282368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1130,6 +1493,1605 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nl-BE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>UltraQueue</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>BufferWrite() Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t/>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>Core I7 920 @ 2,8Ghz</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="800"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>3x2GB 1600-7-7-7</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$O$3:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2846</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4861</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8266</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12962</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12651</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$L$3:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2365</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4890</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7243</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11870</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12972</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12496</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$P$3:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3646</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5868</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8609</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10937</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12506</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$M$3:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1916</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3302</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5414</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7957</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10297</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11538</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11795</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12355</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$Q$3:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1157</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9816</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11055</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12217</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$N$3:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1569</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4840</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7294</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9051</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10502</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11669</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12073</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11291</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="102313984"/>
+        <c:axId val="102315904"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="102313984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Blocksize (Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102315904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102315904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MB/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102313984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="500"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nl-BE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>UltraQueue</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>BufferWrite() Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t/>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>Core I7 920 @ 2,8Ghz</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="800"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>3x2GB 1600-7-7-7</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1Ch - 16kB - (L1 Cache / 2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$T$3:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1519</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2920</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5132</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8306</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12097</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16157</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19458</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21874</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23339</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24453</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1Ch - 128kB - (L2 Cache / 2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$S$3:$S$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>819</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2917</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5074</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8204</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11941</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18103</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17210</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14384</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15212</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1Ch - 256MB - RAM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16k</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32k</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64k</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128k</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>256k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$R$3:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2846</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4861</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8266</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12064</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12810</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12497</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12962</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12651</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="66430464"/>
+        <c:axId val="66531712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="66430464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Blocksize (Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66531712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66531712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MB/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66430464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="nl-BE"/>
   <c:chart>
@@ -1182,8 +3144,152 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="11"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$Q$3:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>419</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$O$3:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="8"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$N$2</c:f>
@@ -1231,7 +3337,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$M$2</c:f>
@@ -1278,8 +3384,56 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="12"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$L$3:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$K$2</c:f>
@@ -1327,7 +3481,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$J$2</c:f>
@@ -1375,7 +3529,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="4"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$I$2</c:f>
@@ -1423,7 +3577,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="5"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$H$2</c:f>
@@ -1471,7 +3625,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="6"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$2</c:f>
@@ -1519,7 +3673,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="7"/>
+          <c:order val="11"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$2</c:f>
@@ -1567,7 +3721,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="8"/>
+          <c:order val="12"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$2</c:f>
@@ -1644,11 +3798,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103074816"/>
-        <c:axId val="103081088"/>
+        <c:axId val="105870080"/>
+        <c:axId val="105872000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103074816"/>
+        <c:axId val="105870080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,14 +3828,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103081088"/>
+        <c:crossAx val="105872000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103081088"/>
+        <c:axId val="105872000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +3861,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103074816"/>
+        <c:crossAx val="105870080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1723,7 +3877,607 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nl-BE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0"/>
+              <a:t>UltraQueue</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0"/>
+              <a:t>BufferWrite() Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0"/>
+              <a:t/>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1" i="0" baseline="0"/>
+              <a:t>Core I7 920 @ 2,8Ghz</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="800" b="1" i="0" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1" i="0" baseline="0"/>
+              <a:t>3x2GB 1600-7-7-7</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-BE" sz="800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$O$3:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 1 Channel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$L$3:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>739</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>419</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 32 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$M$3:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.3 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$Q$3:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v.0.7.2 - 128 Channels</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$N$3:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="105913344"/>
+        <c:axId val="105931904"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="105913344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Blocksize (Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105931904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="105931904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MB/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105913344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="50"/>
+        <c:minorUnit val="10"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="nl-BE"/>
   <c:chart>
@@ -1790,14 +4544,183 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$I$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$38:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4697</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7262</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16516</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16516</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21787</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22260</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21787</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21787</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21787</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16516</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$H$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$38:$H$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1842</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3011</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6598</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8258</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11129</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10893</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$37</c:f>
@@ -1881,7 +4804,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$37</c:f>
@@ -1965,7 +4888,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -2049,7 +4972,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$37</c:f>
@@ -2197,11 +5120,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103411712"/>
-        <c:axId val="103413632"/>
+        <c:axId val="105573760"/>
+        <c:axId val="106317312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103411712"/>
+        <c:axId val="105573760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2222,17 +5145,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103413632"/>
+        <c:crossAx val="106317312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103413632"/>
+        <c:axId val="106317312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2254,24 +5178,26 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103411712"/>
+        <c:crossAx val="105573760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="500"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="nl-BE"/>
   <c:chart>
@@ -2317,14 +5243,111 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$I$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$38:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1338</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$H$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0.7.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$38:$H$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1026</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$G$37</c:f>
@@ -2372,7 +5395,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$F$37</c:f>
@@ -2420,7 +5443,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$E$37</c:f>
@@ -2468,7 +5491,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Blad1!$C$37</c:f>
@@ -2545,11 +5568,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103568128"/>
-        <c:axId val="103570048"/>
+        <c:axId val="106648320"/>
+        <c:axId val="106650240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103568128"/>
+        <c:axId val="106648320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2570,18 +5593,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103570048"/>
+        <c:crossAx val="106650240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103570048"/>
+        <c:axId val="106650240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2603,10 +5627,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103568128"/>
+        <c:crossAx val="106648320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -2614,6 +5639,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2661,6 +5687,42 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2750,6 +5812,87 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9309919" cy="6083710"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9309919" cy="6083710"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9309919" cy="6083710"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -3061,10 +6204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3081,9 +6225,15 @@
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -3091,7 +6241,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3134,8 +6284,26 @@
       <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3178,8 +6346,26 @@
       <c r="N3" s="1">
         <v>1</v>
       </c>
+      <c r="O3" s="1">
+        <v>14</v>
+      </c>
+      <c r="P3" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>14</v>
+      </c>
+      <c r="S3" s="1">
+        <v>14</v>
+      </c>
+      <c r="T3" s="1">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3222,8 +6408,26 @@
       <c r="N4" s="1">
         <v>3</v>
       </c>
+      <c r="O4" s="1">
+        <v>28</v>
+      </c>
+      <c r="P4" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>5</v>
+      </c>
+      <c r="R4" s="1">
+        <v>28</v>
+      </c>
+      <c r="S4" s="1">
+        <v>28</v>
+      </c>
+      <c r="T4" s="1">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3266,8 +6470,26 @@
       <c r="N5" s="1">
         <v>7</v>
       </c>
+      <c r="O5" s="1">
+        <v>55</v>
+      </c>
+      <c r="P5" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>11</v>
+      </c>
+      <c r="R5" s="1">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1">
+        <v>54</v>
+      </c>
+      <c r="T5" s="1">
+        <v>54</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -3310,8 +6532,26 @@
       <c r="N6" s="1">
         <v>16</v>
       </c>
+      <c r="O6" s="1">
+        <v>95</v>
+      </c>
+      <c r="P6" s="1">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>22</v>
+      </c>
+      <c r="R6" s="1">
+        <v>95</v>
+      </c>
+      <c r="S6" s="1">
+        <v>97</v>
+      </c>
+      <c r="T6" s="1">
+        <v>97</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -3354,8 +6594,26 @@
       <c r="N7" s="1">
         <v>31</v>
       </c>
+      <c r="O7" s="1">
+        <v>215</v>
+      </c>
+      <c r="P7" s="1">
+        <v>112</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>46</v>
+      </c>
+      <c r="R7" s="1">
+        <v>215</v>
+      </c>
+      <c r="S7" s="1">
+        <v>218</v>
+      </c>
+      <c r="T7" s="1">
+        <v>218</v>
+      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -3398,8 +6656,26 @@
       <c r="N8" s="1">
         <v>63</v>
       </c>
+      <c r="O8" s="1">
+        <v>421</v>
+      </c>
+      <c r="P8" s="1">
+        <v>221</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>91</v>
+      </c>
+      <c r="R8" s="1">
+        <v>421</v>
+      </c>
+      <c r="S8" s="1">
+        <v>432</v>
+      </c>
+      <c r="T8" s="1">
+        <v>443</v>
+      </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <v>64</v>
       </c>
@@ -3442,8 +6718,26 @@
       <c r="N9" s="1">
         <v>121</v>
       </c>
+      <c r="O9" s="1">
+        <v>800</v>
+      </c>
+      <c r="P9" s="1">
+        <v>419</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>175</v>
+      </c>
+      <c r="R9" s="1">
+        <v>800</v>
+      </c>
+      <c r="S9" s="1">
+        <v>819</v>
+      </c>
+      <c r="T9" s="1">
+        <v>825</v>
+      </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <v>128</v>
       </c>
@@ -3486,8 +6780,26 @@
       <c r="N10" s="1">
         <v>239</v>
       </c>
+      <c r="O10" s="1">
+        <v>1537</v>
+      </c>
+      <c r="P10" s="1">
+        <v>793</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>344</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1537</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1515</v>
+      </c>
+      <c r="T10" s="1">
+        <v>1519</v>
+      </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>256</v>
       </c>
@@ -3530,8 +6842,26 @@
       <c r="N11" s="1">
         <v>466</v>
       </c>
+      <c r="O11" s="1">
+        <v>2846</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1472</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>660</v>
+      </c>
+      <c r="R11" s="1">
+        <v>2846</v>
+      </c>
+      <c r="S11" s="1">
+        <v>2917</v>
+      </c>
+      <c r="T11" s="1">
+        <v>2920</v>
+      </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:20">
       <c r="A12" s="1">
         <v>512</v>
       </c>
@@ -3574,8 +6904,26 @@
       <c r="N12" s="1">
         <v>846</v>
       </c>
+      <c r="O12" s="1">
+        <v>4861</v>
+      </c>
+      <c r="P12" s="1">
+        <v>2197</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1157</v>
+      </c>
+      <c r="R12" s="1">
+        <v>4861</v>
+      </c>
+      <c r="S12" s="1">
+        <v>5074</v>
+      </c>
+      <c r="T12" s="1">
+        <v>5132</v>
+      </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3618,8 +6966,26 @@
       <c r="N13" s="1">
         <v>1569</v>
       </c>
+      <c r="O13" s="1">
+        <v>6954</v>
+      </c>
+      <c r="P13" s="1">
+        <v>3646</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2088</v>
+      </c>
+      <c r="R13" s="1">
+        <v>6954</v>
+      </c>
+      <c r="S13" s="1">
+        <v>8204</v>
+      </c>
+      <c r="T13" s="1">
+        <v>8306</v>
+      </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -3662,8 +7028,26 @@
       <c r="N14" s="1">
         <v>2831</v>
       </c>
+      <c r="O14" s="1">
+        <v>8266</v>
+      </c>
+      <c r="P14" s="1">
+        <v>5868</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>3697</v>
+      </c>
+      <c r="R14" s="1">
+        <v>8266</v>
+      </c>
+      <c r="S14" s="1">
+        <v>11941</v>
+      </c>
+      <c r="T14" s="1">
+        <v>12097</v>
+      </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3706,8 +7090,26 @@
       <c r="N15" s="1">
         <v>4840</v>
       </c>
+      <c r="O15" s="1">
+        <v>10002</v>
+      </c>
+      <c r="P15" s="1">
+        <v>8609</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>5934</v>
+      </c>
+      <c r="R15" s="1">
+        <v>10002</v>
+      </c>
+      <c r="S15" s="1">
+        <v>15003</v>
+      </c>
+      <c r="T15" s="1">
+        <v>16157</v>
+      </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -3750,8 +7152,26 @@
       <c r="N16" s="1">
         <v>7294</v>
       </c>
+      <c r="O16" s="1">
+        <v>12064</v>
+      </c>
+      <c r="P16" s="1">
+        <v>10937</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>8402</v>
+      </c>
+      <c r="R16" s="1">
+        <v>12064</v>
+      </c>
+      <c r="S16" s="1">
+        <v>18103</v>
+      </c>
+      <c r="T16" s="1">
+        <v>20608</v>
+      </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -3794,8 +7214,26 @@
       <c r="N17" s="1">
         <v>9051</v>
       </c>
+      <c r="O17" s="1">
+        <v>12810</v>
+      </c>
+      <c r="P17" s="1">
+        <v>11932</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>9816</v>
+      </c>
+      <c r="R17" s="1">
+        <v>12810</v>
+      </c>
+      <c r="S17" s="1">
+        <v>17210</v>
+      </c>
+      <c r="T17" s="1">
+        <v>19458</v>
+      </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:20">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3838,8 +7276,26 @@
       <c r="N18" s="1">
         <v>10502</v>
       </c>
+      <c r="O18" s="1">
+        <v>12497</v>
+      </c>
+      <c r="P18" s="1">
+        <v>11932</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>11055</v>
+      </c>
+      <c r="R18" s="1">
+        <v>12497</v>
+      </c>
+      <c r="S18" s="1">
+        <v>14384</v>
+      </c>
+      <c r="T18" s="1">
+        <v>21874</v>
+      </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:20">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3882,8 +7338,26 @@
       <c r="N19" s="1">
         <v>11669</v>
       </c>
+      <c r="O19" s="1">
+        <v>12962</v>
+      </c>
+      <c r="P19" s="1">
+        <v>12355</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>12064</v>
+      </c>
+      <c r="R19" s="1">
+        <v>12962</v>
+      </c>
+      <c r="S19" s="1">
+        <v>15003</v>
+      </c>
+      <c r="T19" s="1">
+        <v>23339</v>
+      </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:20">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3926,8 +7400,26 @@
       <c r="N20" s="1">
         <v>12073</v>
       </c>
+      <c r="O20" s="1">
+        <v>12651</v>
+      </c>
+      <c r="P20" s="1">
+        <v>12506</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>12217</v>
+      </c>
+      <c r="R20" s="1">
+        <v>12651</v>
+      </c>
+      <c r="S20" s="1">
+        <v>15212</v>
+      </c>
+      <c r="T20" s="1">
+        <v>24453</v>
+      </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:20">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -3969,6 +7461,24 @@
       </c>
       <c r="N21" s="1">
         <v>11291</v>
+      </c>
+      <c r="O21" s="1">
+        <v>11538</v>
+      </c>
+      <c r="P21" s="1">
+        <v>11669</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>11538</v>
+      </c>
+      <c r="R21" s="1">
+        <v>11538</v>
+      </c>
+      <c r="S21" s="1">
+        <v>15212</v>
+      </c>
+      <c r="T21" s="1">
+        <v>25600</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3993,8 +7503,12 @@
       <c r="G37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="H37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
@@ -4019,8 +7533,12 @@
       <c r="G38" s="1">
         <v>22</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="H38" s="1">
+        <v>23</v>
+      </c>
+      <c r="I38" s="1">
+        <v>23</v>
+      </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10">
@@ -4045,8 +7563,12 @@
       <c r="G39" s="1">
         <v>42</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="H39" s="1">
+        <v>43</v>
+      </c>
+      <c r="I39" s="1">
+        <v>45</v>
+      </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10">
@@ -4071,8 +7593,12 @@
       <c r="G40" s="1">
         <v>80</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="H40" s="1">
+        <v>84</v>
+      </c>
+      <c r="I40" s="1">
+        <v>88</v>
+      </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10">
@@ -4097,8 +7623,12 @@
       <c r="G41" s="1">
         <v>142</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="H41" s="1">
+        <v>145</v>
+      </c>
+      <c r="I41" s="1">
+        <v>165</v>
+      </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10">
@@ -4123,8 +7653,12 @@
       <c r="G42" s="1">
         <v>306</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="H42" s="1">
+        <v>313</v>
+      </c>
+      <c r="I42" s="1">
+        <v>347</v>
+      </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10">
@@ -4149,8 +7683,12 @@
       <c r="G43" s="1">
         <v>528</v>
       </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="H43" s="1">
+        <v>539</v>
+      </c>
+      <c r="I43" s="1">
+        <v>676</v>
+      </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
@@ -4175,8 +7713,12 @@
       <c r="G44" s="1">
         <v>1024</v>
       </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+      <c r="H44" s="1">
+        <v>1026</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1338</v>
+      </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10">
@@ -4201,8 +7743,12 @@
       <c r="G45" s="1">
         <v>1828</v>
       </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
+      <c r="H45" s="1">
+        <v>1842</v>
+      </c>
+      <c r="I45" s="1">
+        <v>2625</v>
+      </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
@@ -4227,8 +7773,12 @@
       <c r="G46" s="1">
         <v>2976</v>
       </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
+      <c r="H46" s="1">
+        <v>3011</v>
+      </c>
+      <c r="I46" s="1">
+        <v>4697</v>
+      </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10">
@@ -4253,8 +7803,12 @@
       <c r="G47" s="1">
         <v>4697</v>
       </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="H47" s="1">
+        <v>4699</v>
+      </c>
+      <c r="I47" s="1">
+        <v>7262</v>
+      </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
@@ -4279,8 +7833,12 @@
       <c r="G48" s="1">
         <v>6564</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
+      <c r="H48" s="1">
+        <v>6598</v>
+      </c>
+      <c r="I48" s="1">
+        <v>9394</v>
+      </c>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10">
@@ -4305,8 +7863,12 @@
       <c r="G49" s="1">
         <v>8258</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="H49" s="1">
+        <v>8258</v>
+      </c>
+      <c r="I49" s="1">
+        <v>16516</v>
+      </c>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
@@ -4331,8 +7893,12 @@
       <c r="G50" s="1">
         <v>10893</v>
       </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="H50" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I50" s="1">
+        <v>16516</v>
+      </c>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10">
@@ -4357,8 +7923,12 @@
       <c r="G51" s="1">
         <v>10893</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="H51" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I51" s="1">
+        <v>21787</v>
+      </c>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
@@ -4383,8 +7953,12 @@
       <c r="G52" s="1">
         <v>10893</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
+      <c r="H52" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I52" s="1">
+        <v>22260</v>
+      </c>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
@@ -4409,8 +7983,12 @@
       <c r="G53" s="1">
         <v>10893</v>
       </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
+      <c r="H53" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I53" s="1">
+        <v>21787</v>
+      </c>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
@@ -4435,8 +8013,12 @@
       <c r="G54" s="1">
         <v>10893</v>
       </c>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
+      <c r="H54" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I54" s="1">
+        <v>21787</v>
+      </c>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
@@ -4461,8 +8043,12 @@
       <c r="G55" s="1">
         <v>11129</v>
       </c>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
+      <c r="H55" s="1">
+        <v>11129</v>
+      </c>
+      <c r="I55" s="1">
+        <v>21787</v>
+      </c>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10">
@@ -4487,8 +8073,12 @@
       <c r="G56" s="1">
         <v>10893</v>
       </c>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
+      <c r="H56" s="1">
+        <v>10893</v>
+      </c>
+      <c r="I56" s="1">
+        <v>16516</v>
+      </c>
       <c r="J56" s="1"/>
     </row>
   </sheetData>

</xml_diff>